<commit_message>
Fix ome tif convert
</commit_message>
<xml_diff>
--- a/examples/annotation_guide.xlsx
+++ b/examples/annotation_guide.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7851" uniqueCount="3230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8229" uniqueCount="3267">
   <si>
     <t xml:space="preserve">Type</t>
   </si>
@@ -9711,6 +9711,135 @@
   </si>
   <si>
     <t xml:space="preserve">CDCA8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T_NK_cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neural</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myeloid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPO+ Mono-Neutrophil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesenchymal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Immature Pericyte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epithelial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endothelial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cycling Stromal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B (Plasma RBC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angiogenic Pericyte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD79B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B Cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cytotoxic/CD8 T Cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T Cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KLRB1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSP90AA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCF7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KCNA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOCK3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UACA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYO10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EFCAB14</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">myofibroblast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (RSPO2+)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Myofibroblast (RSPO2+)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MACIR (C5orf30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proliferating Erythrocytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIHBP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GJA4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MRGPRX2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fibroblast </t>
   </si>
 </sst>
 </file>
@@ -9720,7 +9849,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -9755,13 +9884,50 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8FAADC"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7E7"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF9C0006"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -9798,7 +9964,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -9815,6 +9981,34 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9824,6 +10018,81 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF9C0006"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB4C7E7"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF8FAADC"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFC7CE"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -9834,8 +10103,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A628" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A632" activeCellId="0" sqref="A632"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3848" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3871" activeCellId="0" sqref="E3871"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -41249,6 +41518,1518 @@
       </c>
       <c r="B3926" s="2" t="s">
         <v>3209</v>
+      </c>
+    </row>
+    <row r="3927" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3927" s="4" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B3927" s="4" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="3928" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3928" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="B3928" s="4" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="3929" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3929" s="4" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B3929" s="4" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="3930" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3930" s="4" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B3930" s="4" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="3931" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3931" s="4" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B3931" s="4" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="3932" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3932" s="4" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B3932" s="4" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="3933" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3933" s="5" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B3933" s="5" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="3934" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3934" s="4" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B3934" s="4" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="3935" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3935" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="B3935" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="3936" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3936" s="4" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B3936" s="4" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="3937" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3937" s="4" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B3937" s="4" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="3938" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3938" s="4" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B3938" s="4" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="3939" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3939" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3939" s="4" t="s">
+        <v>2645</v>
+      </c>
+    </row>
+    <row r="3940" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3940" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="B3940" s="6" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="3941" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3941" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3941" s="7" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="3942" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3942" s="4" t="s">
+        <v>981</v>
+      </c>
+      <c r="B3942" s="8" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="3943" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3943" s="4" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B3943" s="8" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="3944" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3944" s="4" t="s">
+        <v>2355</v>
+      </c>
+      <c r="B3944" s="4" t="s">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="3945" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3945" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B3945" s="4" t="s">
+        <v>3233</v>
+      </c>
+    </row>
+    <row r="3946" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3946" s="4" t="s">
+        <v>2579</v>
+      </c>
+      <c r="B3946" s="4" t="s">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="3947" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3947" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="B3947" s="4" t="s">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="3948" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3948" s="4" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B3948" s="4" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="3949" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3949" s="4" t="s">
+        <v>842</v>
+      </c>
+      <c r="B3949" s="4" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="3950" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3950" s="4" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B3950" s="4" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="3951" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3951" s="4" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B3951" s="4" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="3952" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3952" s="4" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B3952" s="4" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="3953" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3953" s="4" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B3953" s="4" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="3954" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3954" s="4" t="s">
+        <v>2381</v>
+      </c>
+      <c r="B3954" s="4" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="3955" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3955" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="B3955" s="4" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="3956" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3956" s="4" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B3956" s="4" t="s">
+        <v>3235</v>
+      </c>
+    </row>
+    <row r="3957" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3957" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="B3957" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="3958" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3958" s="4" t="s">
+        <v>674</v>
+      </c>
+      <c r="B3958" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="3959" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3959" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3959" s="4" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="3960" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3960" s="4" t="s">
+        <v>3142</v>
+      </c>
+      <c r="B3960" s="4" t="s">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="3961" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3961" s="4" t="s">
+        <v>960</v>
+      </c>
+      <c r="B3961" s="4" t="s">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="3962" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3962" s="4" t="s">
+        <v>1851</v>
+      </c>
+      <c r="B3962" s="4" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="3963" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3963" s="4" t="s">
+        <v>2640</v>
+      </c>
+      <c r="B3963" s="4" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="3964" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3964" s="4" t="s">
+        <v>2622</v>
+      </c>
+      <c r="B3964" s="4" t="s">
+        <v>2603</v>
+      </c>
+    </row>
+    <row r="3965" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3965" s="4" t="s">
+        <v>1870</v>
+      </c>
+      <c r="B3965" s="4" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="3966" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3966" s="4" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B3966" s="4" t="s">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="3967" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3967" s="4" t="s">
+        <v>3241</v>
+      </c>
+      <c r="B3967" s="4" t="s">
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="3968" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3968" s="4" t="s">
+        <v>844</v>
+      </c>
+      <c r="B3968" s="4" t="s">
+        <v>3242</v>
+      </c>
+    </row>
+    <row r="3969" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3969" s="4" t="s">
+        <v>2647</v>
+      </c>
+      <c r="B3969" s="4" t="s">
+        <v>3243</v>
+      </c>
+    </row>
+    <row r="3970" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3970" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="B3970" s="4" t="s">
+        <v>3243</v>
+      </c>
+    </row>
+    <row r="3971" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3971" s="4" t="s">
+        <v>3244</v>
+      </c>
+      <c r="B3971" s="4" t="s">
+        <v>3245</v>
+      </c>
+    </row>
+    <row r="3972" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3972" s="4" t="s">
+        <v>1843</v>
+      </c>
+      <c r="B3972" s="4" t="s">
+        <v>3245</v>
+      </c>
+    </row>
+    <row r="3973" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3973" s="4" t="s">
+        <v>3246</v>
+      </c>
+      <c r="B3973" s="4" t="s">
+        <v>3245</v>
+      </c>
+    </row>
+    <row r="3974" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3974" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="B3974" s="4" t="s">
+        <v>3247</v>
+      </c>
+    </row>
+    <row r="3975" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3975" s="4" t="s">
+        <v>3248</v>
+      </c>
+      <c r="B3975" s="4" t="s">
+        <v>3247</v>
+      </c>
+    </row>
+    <row r="3976" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3976" s="4" t="s">
+        <v>2552</v>
+      </c>
+      <c r="B3976" s="4" t="s">
+        <v>3247</v>
+      </c>
+    </row>
+    <row r="3977" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3977" s="4" t="s">
+        <v>3249</v>
+      </c>
+      <c r="B3977" s="4" t="s">
+        <v>3247</v>
+      </c>
+    </row>
+    <row r="3978" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3978" s="4" t="s">
+        <v>773</v>
+      </c>
+      <c r="B3978" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="3979" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3979" s="4" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B3979" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="3980" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3980" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3980" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="3981" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3981" s="4" t="s">
+        <v>3250</v>
+      </c>
+      <c r="B3981" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="3982" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3982" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B3982" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="3983" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3983" s="4" t="s">
+        <v>3251</v>
+      </c>
+      <c r="B3983" s="4" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="3984" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3984" s="4" t="s">
+        <v>3252</v>
+      </c>
+      <c r="B3984" s="4" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="3985" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3985" s="4" t="s">
+        <v>3253</v>
+      </c>
+      <c r="B3985" s="4" t="s">
+        <v>3254</v>
+      </c>
+    </row>
+    <row r="3986" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3986" s="4" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B3986" s="4" t="s">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="3987" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3987" s="4" t="s">
+        <v>1647</v>
+      </c>
+      <c r="B3987" s="4" t="s">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="3988" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3988" s="4" t="s">
+        <v>1867</v>
+      </c>
+      <c r="B3988" s="4" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="3989" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3989" s="4" t="s">
+        <v>1868</v>
+      </c>
+      <c r="B3989" s="4" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="3990" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3990" s="4" t="s">
+        <v>1871</v>
+      </c>
+      <c r="B3990" s="4" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="3991" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3991" s="4" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B3991" s="4" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="3992" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3992" s="4" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B3992" s="4" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="3993" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3993" s="4" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B3993" s="4" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="3994" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3994" s="4" t="s">
+        <v>1869</v>
+      </c>
+      <c r="B3994" s="4" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="3995" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3995" s="4" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B3995" s="4" t="s">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="3996" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3996" s="4" t="s">
+        <v>2602</v>
+      </c>
+      <c r="B3996" s="4" t="s">
+        <v>2603</v>
+      </c>
+    </row>
+    <row r="3997" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3997" s="4" t="s">
+        <v>2604</v>
+      </c>
+      <c r="B3997" s="4" t="s">
+        <v>2603</v>
+      </c>
+    </row>
+    <row r="3998" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3998" s="4" t="s">
+        <v>2644</v>
+      </c>
+      <c r="B3998" s="4" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="3999" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3999" s="4" t="s">
+        <v>740</v>
+      </c>
+      <c r="B3999" s="4" t="s">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="4000" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4000" s="4" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B4000" s="4" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="4001" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4001" s="4" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B4001" s="4" t="s">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="4002" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4002" s="4" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B4002" s="4" t="s">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="4003" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4003" s="4" t="s">
+        <v>3255</v>
+      </c>
+      <c r="B4003" s="4" t="s">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="4004" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4004" s="4" t="s">
+        <v>3256</v>
+      </c>
+      <c r="B4004" s="4" t="s">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="4005" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4005" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4005" s="4" t="s">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="4006" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4006" s="4" t="s">
+        <v>3257</v>
+      </c>
+      <c r="B4006" s="4" t="s">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="4007" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4007" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4007" s="4" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="4008" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4008" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4008" s="4" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="4009" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4009" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4009" s="4" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="4010" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4010" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4010" s="4" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="4011" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4011" s="4" t="s">
+        <v>672</v>
+      </c>
+      <c r="B4011" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="4012" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4012" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="B4012" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="4013" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4013" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="B4013" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="4014" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4014" s="4" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B4014" s="4" t="s">
+        <v>3235</v>
+      </c>
+    </row>
+    <row r="4015" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4015" s="4" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B4015" s="4" t="s">
+        <v>3235</v>
+      </c>
+    </row>
+    <row r="4016" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4016" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4016" s="4" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="4017" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4017" s="4" t="s">
+        <v>787</v>
+      </c>
+      <c r="B4017" s="4" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="4018" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4018" s="4" t="s">
+        <v>2379</v>
+      </c>
+      <c r="B4018" s="4" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="4019" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4019" s="4" t="s">
+        <v>2133</v>
+      </c>
+      <c r="B4019" s="4" t="s">
+        <v>2380</v>
+      </c>
+    </row>
+    <row r="4020" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4020" s="4" t="s">
+        <v>2476</v>
+      </c>
+      <c r="B4020" s="4" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="4021" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4021" s="4" t="s">
+        <v>2491</v>
+      </c>
+      <c r="B4021" s="4" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="4022" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4022" s="4" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B4022" s="4" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="4023" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4023" s="4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B4023" s="4" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="4024" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4024" s="4" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B4024" s="4" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="4025" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4025" s="4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B4025" s="4" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="4026" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4026" s="4" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B4026" s="4" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="4027" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4027" s="4" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B4027" s="4" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="4028" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4028" s="4" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B4028" s="4" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="4029" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4029" s="4" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B4029" s="4" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="4030" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4030" s="4" t="s">
+        <v>1709</v>
+      </c>
+      <c r="B4030" s="4" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="4031" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4031" s="4" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B4031" s="4" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="4032" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4032" s="4" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B4032" s="4" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="4033" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4033" s="4" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B4033" s="4" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="4034" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4034" s="4" t="s">
+        <v>2411</v>
+      </c>
+      <c r="B4034" s="4" t="s">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="4035" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4035" s="4" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B4035" s="4" t="s">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="4036" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4036" s="4" t="s">
+        <v>2601</v>
+      </c>
+      <c r="B4036" s="4" t="s">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="4037" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4037" s="4" t="s">
+        <v>2443</v>
+      </c>
+      <c r="B4037" s="4" t="s">
+        <v>3233</v>
+      </c>
+    </row>
+    <row r="4038" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4038" s="4" t="s">
+        <v>2451</v>
+      </c>
+      <c r="B4038" s="4" t="s">
+        <v>3233</v>
+      </c>
+    </row>
+    <row r="4039" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4039" s="4" t="s">
+        <v>2356</v>
+      </c>
+      <c r="B4039" s="4" t="s">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="4040" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4040" s="4" t="s">
+        <v>2349</v>
+      </c>
+      <c r="B4040" s="4" t="s">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="4041" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4041" s="4" t="s">
+        <v>2352</v>
+      </c>
+      <c r="B4041" s="4" t="s">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="4042" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4042" s="4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B4042" s="4" t="s">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="4043" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4043" s="4" t="s">
+        <v>2357</v>
+      </c>
+      <c r="B4043" s="4" t="s">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="4044" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4044" s="4" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B4044" s="8" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="4045" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4045" s="4" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B4045" s="8" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="4046" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4046" s="4" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B4046" s="8" t="s">
+        <v>3258</v>
+      </c>
+    </row>
+    <row r="4047" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4047" s="4" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B4047" s="4" t="s">
+        <v>3259</v>
+      </c>
+    </row>
+    <row r="4048" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4048" s="4" t="s">
+        <v>829</v>
+      </c>
+      <c r="B4048" s="4" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="4049" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4049" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="B4049" s="4" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="4050" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4050" s="4" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B4050" s="4" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="4051" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4051" s="4" t="s">
+        <v>3111</v>
+      </c>
+      <c r="B4051" s="4" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="4052" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4052" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="B4052" s="6" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="4053" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4053" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B4053" s="4" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="4054" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4054" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="B4054" s="4" t="s">
+        <v>2645</v>
+      </c>
+    </row>
+    <row r="4055" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4055" s="4" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B4055" s="4" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="4056" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4056" s="4" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B4056" s="4" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="4057" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4057" s="4" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B4057" s="4" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="4058" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4058" s="4" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B4058" s="4" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="4059" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4059" s="9" t="s">
+        <v>3260</v>
+      </c>
+      <c r="B4059" s="4" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="4060" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4060" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B4060" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="4061" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4061" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B4061" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="4062" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4062" s="4" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B4062" s="4" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="4063" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4063" s="4" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B4063" s="4" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="4064" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4064" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="B4064" s="4" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="4065" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4065" s="4" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B4065" s="4" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="4066" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4066" s="4" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B4066" s="4" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="4067" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4067" s="4" t="s">
+        <v>1510</v>
+      </c>
+      <c r="B4067" s="4" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="4068" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4068" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4068" s="4" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="4069" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4069" s="4" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B4069" s="4" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="4070" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4070" s="4" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B4070" s="4" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="4071" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4071" s="4" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B4071" s="4" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="4072" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4072" s="4" t="s">
+        <v>1545</v>
+      </c>
+      <c r="B4072" s="4" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="4073" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4073" s="4" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B4073" s="4" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="4074" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4074" s="4" t="s">
+        <v>810</v>
+      </c>
+      <c r="B4074" s="4" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="4075" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4075" s="4" t="s">
+        <v>817</v>
+      </c>
+      <c r="B4075" s="4" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="4076" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4076" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="B4076" s="4" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="4077" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4077" s="4" t="s">
+        <v>815</v>
+      </c>
+      <c r="B4077" s="4" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="4078" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4078" s="4" t="s">
+        <v>813</v>
+      </c>
+      <c r="B4078" s="4" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="4079" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4079" s="4" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B4079" s="4" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="4080" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4080" s="4" t="s">
+        <v>1598</v>
+      </c>
+      <c r="B4080" s="4" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="4081" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4081" s="4" t="s">
+        <v>2257</v>
+      </c>
+      <c r="B4081" s="4" t="s">
+        <v>3261</v>
+      </c>
+    </row>
+    <row r="4082" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4082" s="4" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B4082" s="4" t="s">
+        <v>3261</v>
+      </c>
+    </row>
+    <row r="4083" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4083" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4083" s="4" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="4084" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4084" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4084" s="4" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="4085" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4085" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4085" s="4" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="4086" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4086" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4086" s="4" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="4087" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4087" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4087" s="4" t="s">
+        <v>3236</v>
+      </c>
+    </row>
+    <row r="4088" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4088" s="4" t="s">
+        <v>3262</v>
+      </c>
+      <c r="B4088" s="4" t="s">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="4089" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4089" s="4" t="s">
+        <v>3263</v>
+      </c>
+      <c r="B4089" s="4" t="s">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="4090" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4090" s="4" t="s">
+        <v>3264</v>
+      </c>
+      <c r="B4090" s="4" t="s">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="4091" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4091" s="4" t="s">
+        <v>3012</v>
+      </c>
+      <c r="B4091" s="4" t="s">
+        <v>3237</v>
+      </c>
+    </row>
+    <row r="4092" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4092" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B4092" s="4" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="4093" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4093" s="4" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B4093" s="4" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="4094" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4094" s="4" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B4094" s="4" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="4095" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4095" s="4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B4095" s="4" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="4096" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4096" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="B4096" s="4" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="4097" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4097" s="4" t="s">
+        <v>2350</v>
+      </c>
+      <c r="B4097" s="4" t="s">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="4098" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4098" s="4" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B4098" s="4" t="s">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="4099" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4099" s="4" t="s">
+        <v>2351</v>
+      </c>
+      <c r="B4099" s="4" t="s">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="4100" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4100" s="4" t="s">
+        <v>3145</v>
+      </c>
+      <c r="B4100" s="4" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="4101" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4101" s="4" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B4101" s="4" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="4102" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4102" s="4" t="s">
+        <v>2856</v>
+      </c>
+      <c r="B4102" s="4" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="4103" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4103" s="4" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B4103" s="4" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="4104" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4104" s="4" t="s">
+        <v>3022</v>
+      </c>
+      <c r="B4104" s="4" t="s">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="4105" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4105" s="4" t="s">
+        <v>812</v>
+      </c>
+      <c r="B4105" s="4" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="4106" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4106" s="4" t="s">
+        <v>814</v>
+      </c>
+      <c r="B4106" s="4" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="4107" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4107" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="B4107" s="4" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="4108" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4108" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="B4108" s="4" t="s">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="4109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4109" s="10" t="s">
+        <v>3265</v>
+      </c>
+      <c r="B4109" s="10" t="s">
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="4110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4110" s="10" t="s">
+        <v>2513</v>
+      </c>
+      <c r="B4110" s="10" t="s">
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="4111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4111" s="10" t="s">
+        <v>2523</v>
+      </c>
+      <c r="B4111" s="10" t="s">
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="4112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4112" s="10" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B4112" s="10" t="s">
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="4113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4113" s="10" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B4113" s="10" t="s">
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="4114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4114" s="10" t="s">
+        <v>2517</v>
+      </c>
+      <c r="B4114" s="10" t="s">
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="4115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4115" s="10" t="s">
+        <v>2069</v>
+      </c>
+      <c r="B4115" s="10" t="s">
+        <v>2511</v>
       </c>
     </row>
     <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -41366,6 +43147,9 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <conditionalFormatting sqref="A3927:A4108">
+    <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -41387,7 +43171,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>